<commit_message>
set status to complete for all units
</commit_message>
<xml_diff>
--- a/validation/policy_coverage_test_case_list.xlsx
+++ b/validation/policy_coverage_test_case_list.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25128"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26924"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="\\wsl$\Ubuntu-20.04\home\joh\dev\OasisLMF_backallocation\validation\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="\\wsl$\Ubuntu-20.04\home\joh\dev\OasisLMF_fm_pol_cov_tests\validation\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8274C426-B54D-4FE8-B38A-DCDD499AB5D3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4C214F8B-C412-4765-AB8F-7D51F00E286D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="22932" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -118,9 +118,6 @@
     <t>PolLimit1Building</t>
   </si>
   <si>
-    <t>In progress</t>
-  </si>
-  <si>
     <t>PolMinDed4BI</t>
   </si>
   <si>
@@ -227,6 +224,9 @@
   </si>
   <si>
     <t>LocDed3Limit</t>
+  </si>
+  <si>
+    <t>complete</t>
   </si>
 </sst>
 </file>
@@ -1069,53 +1069,53 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:AJ26"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
-      <selection activeCell="A2" sqref="A2"/>
+    <sheetView tabSelected="1" topLeftCell="V1" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
+      <selection activeCell="AJ3" sqref="AJ3:AJ26"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="9.7109375" customWidth="1"/>
-    <col min="2" max="2" width="16.5703125" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="12.85546875" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="10.85546875" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="11.7109375" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="15.85546875" bestFit="1" customWidth="1"/>
-    <col min="7" max="8" width="15.85546875" customWidth="1"/>
-    <col min="9" max="9" width="16.7109375" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="10.140625" bestFit="1" customWidth="1"/>
-    <col min="11" max="12" width="10.140625" customWidth="1"/>
+    <col min="1" max="1" width="9.6640625" customWidth="1"/>
+    <col min="2" max="2" width="16.5546875" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="12.88671875" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="10.88671875" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="11.6640625" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="15.88671875" bestFit="1" customWidth="1"/>
+    <col min="7" max="8" width="15.88671875" customWidth="1"/>
+    <col min="9" max="9" width="16.6640625" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="10.109375" bestFit="1" customWidth="1"/>
+    <col min="11" max="12" width="10.109375" customWidth="1"/>
     <col min="13" max="13" width="11" bestFit="1" customWidth="1"/>
-    <col min="14" max="14" width="10.85546875" bestFit="1" customWidth="1"/>
-    <col min="15" max="16" width="10.85546875" customWidth="1"/>
-    <col min="17" max="17" width="11.7109375" bestFit="1" customWidth="1"/>
-    <col min="18" max="18" width="11.7109375" customWidth="1"/>
-    <col min="19" max="19" width="16.140625" bestFit="1" customWidth="1"/>
-    <col min="20" max="20" width="12.5703125" bestFit="1" customWidth="1"/>
-    <col min="21" max="21" width="13.5703125" bestFit="1" customWidth="1"/>
-    <col min="22" max="22" width="19.42578125" bestFit="1" customWidth="1"/>
-    <col min="23" max="23" width="19.7109375" bestFit="1" customWidth="1"/>
-    <col min="24" max="24" width="15.85546875" bestFit="1" customWidth="1"/>
-    <col min="25" max="25" width="16.7109375" bestFit="1" customWidth="1"/>
-    <col min="26" max="26" width="19.42578125" bestFit="1" customWidth="1"/>
-    <col min="27" max="27" width="19.7109375" bestFit="1" customWidth="1"/>
-    <col min="28" max="28" width="15.85546875" bestFit="1" customWidth="1"/>
-    <col min="29" max="29" width="16.7109375" bestFit="1" customWidth="1"/>
-    <col min="30" max="30" width="19.42578125" bestFit="1" customWidth="1"/>
-    <col min="31" max="31" width="19.7109375" bestFit="1" customWidth="1"/>
-    <col min="32" max="32" width="15.85546875" bestFit="1" customWidth="1"/>
-    <col min="33" max="33" width="16.7109375" bestFit="1" customWidth="1"/>
-    <col min="34" max="34" width="16.7109375" customWidth="1"/>
-    <col min="35" max="35" width="10.28515625" bestFit="1" customWidth="1"/>
-    <col min="36" max="36" width="9.7109375" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="10.88671875" bestFit="1" customWidth="1"/>
+    <col min="15" max="16" width="10.88671875" customWidth="1"/>
+    <col min="17" max="17" width="11.6640625" bestFit="1" customWidth="1"/>
+    <col min="18" max="18" width="11.6640625" customWidth="1"/>
+    <col min="19" max="19" width="16.109375" bestFit="1" customWidth="1"/>
+    <col min="20" max="20" width="12.5546875" bestFit="1" customWidth="1"/>
+    <col min="21" max="21" width="13.5546875" bestFit="1" customWidth="1"/>
+    <col min="22" max="22" width="19.44140625" bestFit="1" customWidth="1"/>
+    <col min="23" max="23" width="19.6640625" bestFit="1" customWidth="1"/>
+    <col min="24" max="24" width="15.88671875" bestFit="1" customWidth="1"/>
+    <col min="25" max="25" width="16.6640625" bestFit="1" customWidth="1"/>
+    <col min="26" max="26" width="19.44140625" bestFit="1" customWidth="1"/>
+    <col min="27" max="27" width="19.6640625" bestFit="1" customWidth="1"/>
+    <col min="28" max="28" width="15.88671875" bestFit="1" customWidth="1"/>
+    <col min="29" max="29" width="16.6640625" bestFit="1" customWidth="1"/>
+    <col min="30" max="30" width="19.44140625" bestFit="1" customWidth="1"/>
+    <col min="31" max="31" width="19.6640625" bestFit="1" customWidth="1"/>
+    <col min="32" max="32" width="15.88671875" bestFit="1" customWidth="1"/>
+    <col min="33" max="33" width="16.6640625" bestFit="1" customWidth="1"/>
+    <col min="34" max="34" width="16.6640625" customWidth="1"/>
+    <col min="35" max="35" width="10.33203125" bestFit="1" customWidth="1"/>
+    <col min="36" max="36" width="9.6640625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:36" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:36" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
-        <v>63</v>
-      </c>
-    </row>
-    <row r="2" spans="1:36" x14ac:dyDescent="0.25">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="2" spans="1:36" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
         <v>0</v>
       </c>
@@ -1123,7 +1123,7 @@
         <v>1</v>
       </c>
       <c r="C2" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="D2" t="s">
         <v>2</v>
@@ -1171,10 +1171,10 @@
         <v>4</v>
       </c>
       <c r="S2" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="T2" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="U2" t="s">
         <v>5</v>
@@ -1192,28 +1192,28 @@
         <v>27</v>
       </c>
       <c r="Z2" t="s">
+        <v>28</v>
+      </c>
+      <c r="AA2" t="s">
         <v>29</v>
       </c>
-      <c r="AA2" t="s">
+      <c r="AB2" t="s">
         <v>30</v>
       </c>
-      <c r="AB2" t="s">
+      <c r="AC2" t="s">
         <v>31</v>
       </c>
-      <c r="AC2" t="s">
+      <c r="AD2" t="s">
         <v>32</v>
       </c>
-      <c r="AD2" t="s">
+      <c r="AE2" t="s">
         <v>33</v>
       </c>
-      <c r="AE2" t="s">
+      <c r="AF2" t="s">
         <v>34</v>
       </c>
-      <c r="AF2" t="s">
+      <c r="AG2" t="s">
         <v>35</v>
-      </c>
-      <c r="AG2" t="s">
-        <v>36</v>
       </c>
       <c r="AH2" t="s">
         <v>6</v>
@@ -1225,533 +1225,533 @@
         <v>8</v>
       </c>
     </row>
-    <row r="3" spans="1:36" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:36" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
+        <v>38</v>
+      </c>
+      <c r="B3" t="s">
+        <v>9</v>
+      </c>
+      <c r="C3" t="s">
+        <v>9</v>
+      </c>
+      <c r="D3" t="s">
+        <v>9</v>
+      </c>
+      <c r="E3" t="s">
+        <v>9</v>
+      </c>
+      <c r="X3" t="s">
+        <v>9</v>
+      </c>
+      <c r="AH3" t="s">
+        <v>10</v>
+      </c>
+      <c r="AI3" t="s">
+        <v>11</v>
+      </c>
+      <c r="AJ3" t="s">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="4" spans="1:36" x14ac:dyDescent="0.3">
+      <c r="A4" t="s">
         <v>39</v>
       </c>
-      <c r="B3" t="s">
-        <v>9</v>
-      </c>
-      <c r="C3" t="s">
-        <v>9</v>
-      </c>
-      <c r="D3" t="s">
-        <v>9</v>
-      </c>
-      <c r="E3" t="s">
-        <v>9</v>
-      </c>
-      <c r="X3" t="s">
-        <v>9</v>
-      </c>
-      <c r="AH3" t="s">
-        <v>10</v>
-      </c>
-      <c r="AI3" t="s">
-        <v>11</v>
-      </c>
-      <c r="AJ3" t="s">
-        <v>28</v>
-      </c>
-    </row>
-    <row r="4" spans="1:36" x14ac:dyDescent="0.25">
-      <c r="A4" t="s">
+      <c r="D4" t="s">
+        <v>9</v>
+      </c>
+      <c r="V4" t="s">
+        <v>9</v>
+      </c>
+      <c r="AH4" t="s">
+        <v>10</v>
+      </c>
+      <c r="AI4" t="s">
+        <v>11</v>
+      </c>
+      <c r="AJ4" t="s">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="5" spans="1:36" x14ac:dyDescent="0.3">
+      <c r="A5" t="s">
         <v>40</v>
       </c>
-      <c r="D4" t="s">
-        <v>9</v>
-      </c>
-      <c r="V4" t="s">
-        <v>9</v>
-      </c>
-      <c r="AH4" t="s">
-        <v>10</v>
-      </c>
-      <c r="AI4" t="s">
-        <v>11</v>
-      </c>
-      <c r="AJ4" t="s">
-        <v>28</v>
-      </c>
-    </row>
-    <row r="5" spans="1:36" x14ac:dyDescent="0.25">
-      <c r="A5" t="s">
+      <c r="D5" t="s">
+        <v>9</v>
+      </c>
+      <c r="W5" t="s">
+        <v>9</v>
+      </c>
+      <c r="AH5" t="s">
+        <v>10</v>
+      </c>
+      <c r="AI5" t="s">
+        <v>11</v>
+      </c>
+      <c r="AJ5" t="s">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="6" spans="1:36" x14ac:dyDescent="0.3">
+      <c r="A6" t="s">
         <v>41</v>
       </c>
-      <c r="D5" t="s">
-        <v>9</v>
-      </c>
-      <c r="W5" t="s">
-        <v>9</v>
-      </c>
-      <c r="AH5" t="s">
-        <v>10</v>
-      </c>
-      <c r="AI5" t="s">
-        <v>11</v>
-      </c>
-      <c r="AJ5" t="s">
-        <v>28</v>
-      </c>
-    </row>
-    <row r="6" spans="1:36" x14ac:dyDescent="0.25">
-      <c r="A6" t="s">
+      <c r="D6" t="s">
+        <v>9</v>
+      </c>
+      <c r="AB6" t="s">
+        <v>9</v>
+      </c>
+      <c r="AF6" t="s">
+        <v>9</v>
+      </c>
+      <c r="AH6" t="s">
+        <v>10</v>
+      </c>
+      <c r="AI6" t="s">
+        <v>11</v>
+      </c>
+      <c r="AJ6" t="s">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="7" spans="1:36" x14ac:dyDescent="0.3">
+      <c r="A7" t="s">
         <v>42</v>
       </c>
-      <c r="D6" t="s">
-        <v>9</v>
-      </c>
-      <c r="AB6" t="s">
-        <v>9</v>
-      </c>
-      <c r="AF6" t="s">
-        <v>9</v>
-      </c>
-      <c r="AH6" t="s">
-        <v>10</v>
-      </c>
-      <c r="AI6" t="s">
-        <v>11</v>
-      </c>
-      <c r="AJ6" t="s">
-        <v>28</v>
-      </c>
-    </row>
-    <row r="7" spans="1:36" x14ac:dyDescent="0.25">
-      <c r="A7" t="s">
+      <c r="D7" t="s">
+        <v>9</v>
+      </c>
+      <c r="Z7" t="s">
+        <v>9</v>
+      </c>
+      <c r="AD7" t="s">
+        <v>9</v>
+      </c>
+      <c r="AH7" t="s">
+        <v>10</v>
+      </c>
+      <c r="AI7" t="s">
+        <v>11</v>
+      </c>
+      <c r="AJ7" t="s">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="8" spans="1:36" x14ac:dyDescent="0.3">
+      <c r="A8" t="s">
         <v>43</v>
       </c>
-      <c r="D7" t="s">
-        <v>9</v>
-      </c>
-      <c r="Z7" t="s">
-        <v>9</v>
-      </c>
-      <c r="AD7" t="s">
-        <v>9</v>
-      </c>
-      <c r="AH7" t="s">
-        <v>10</v>
-      </c>
-      <c r="AI7" t="s">
-        <v>11</v>
-      </c>
-      <c r="AJ7" t="s">
-        <v>28</v>
-      </c>
-    </row>
-    <row r="8" spans="1:36" x14ac:dyDescent="0.25">
-      <c r="A8" t="s">
+      <c r="D8" t="s">
+        <v>9</v>
+      </c>
+      <c r="AA8" t="s">
+        <v>9</v>
+      </c>
+      <c r="AE8" t="s">
+        <v>9</v>
+      </c>
+      <c r="AH8" t="s">
+        <v>10</v>
+      </c>
+      <c r="AI8" t="s">
+        <v>11</v>
+      </c>
+      <c r="AJ8" t="s">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="9" spans="1:36" x14ac:dyDescent="0.3">
+      <c r="A9" t="s">
         <v>44</v>
       </c>
-      <c r="D8" t="s">
-        <v>9</v>
-      </c>
-      <c r="AA8" t="s">
-        <v>9</v>
-      </c>
-      <c r="AE8" t="s">
-        <v>9</v>
-      </c>
-      <c r="AH8" t="s">
-        <v>10</v>
-      </c>
-      <c r="AI8" t="s">
-        <v>11</v>
-      </c>
-      <c r="AJ8" t="s">
-        <v>28</v>
-      </c>
-    </row>
-    <row r="9" spans="1:36" x14ac:dyDescent="0.25">
-      <c r="A9" t="s">
+      <c r="D9" t="s">
+        <v>9</v>
+      </c>
+      <c r="Y9" t="s">
+        <v>9</v>
+      </c>
+      <c r="AH9" t="s">
+        <v>10</v>
+      </c>
+      <c r="AI9" t="s">
+        <v>11</v>
+      </c>
+      <c r="AJ9" t="s">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="10" spans="1:36" x14ac:dyDescent="0.3">
+      <c r="A10" t="s">
         <v>45</v>
       </c>
-      <c r="D9" t="s">
-        <v>9</v>
-      </c>
-      <c r="Y9" t="s">
-        <v>9</v>
-      </c>
-      <c r="AH9" t="s">
-        <v>10</v>
-      </c>
-      <c r="AI9" t="s">
-        <v>11</v>
-      </c>
-      <c r="AJ9" t="s">
-        <v>28</v>
-      </c>
-    </row>
-    <row r="10" spans="1:36" x14ac:dyDescent="0.25">
-      <c r="A10" t="s">
+      <c r="D10" t="s">
+        <v>9</v>
+      </c>
+      <c r="AC10" t="s">
+        <v>9</v>
+      </c>
+      <c r="AG10" t="s">
+        <v>9</v>
+      </c>
+      <c r="AH10" t="s">
+        <v>10</v>
+      </c>
+      <c r="AI10" t="s">
+        <v>11</v>
+      </c>
+      <c r="AJ10" t="s">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="11" spans="1:36" x14ac:dyDescent="0.3">
+      <c r="A11" t="s">
         <v>46</v>
       </c>
-      <c r="D10" t="s">
-        <v>9</v>
-      </c>
-      <c r="AC10" t="s">
-        <v>9</v>
-      </c>
-      <c r="AG10" t="s">
-        <v>9</v>
-      </c>
-      <c r="AH10" t="s">
-        <v>10</v>
-      </c>
-      <c r="AI10" t="s">
-        <v>11</v>
-      </c>
-      <c r="AJ10" t="s">
-        <v>28</v>
-      </c>
-    </row>
-    <row r="11" spans="1:36" x14ac:dyDescent="0.25">
-      <c r="A11" t="s">
+      <c r="D11" t="s">
+        <v>9</v>
+      </c>
+      <c r="H11" t="s">
+        <v>9</v>
+      </c>
+      <c r="AH11" t="s">
+        <v>10</v>
+      </c>
+      <c r="AI11" t="s">
+        <v>11</v>
+      </c>
+      <c r="AJ11" t="s">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="12" spans="1:36" x14ac:dyDescent="0.3">
+      <c r="A12" t="s">
         <v>47</v>
       </c>
-      <c r="D11" t="s">
-        <v>9</v>
-      </c>
-      <c r="H11" t="s">
-        <v>9</v>
-      </c>
-      <c r="AH11" t="s">
-        <v>10</v>
-      </c>
-      <c r="AI11" t="s">
-        <v>11</v>
-      </c>
-      <c r="AJ11" t="s">
-        <v>28</v>
-      </c>
-    </row>
-    <row r="12" spans="1:36" x14ac:dyDescent="0.25">
-      <c r="A12" t="s">
+      <c r="D12" t="s">
+        <v>9</v>
+      </c>
+      <c r="F12" t="s">
+        <v>9</v>
+      </c>
+      <c r="AH12" t="s">
+        <v>10</v>
+      </c>
+      <c r="AI12" t="s">
+        <v>11</v>
+      </c>
+      <c r="AJ12" t="s">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="13" spans="1:36" x14ac:dyDescent="0.3">
+      <c r="A13" t="s">
         <v>48</v>
       </c>
-      <c r="D12" t="s">
-        <v>9</v>
-      </c>
-      <c r="F12" t="s">
-        <v>9</v>
-      </c>
-      <c r="AH12" t="s">
-        <v>10</v>
-      </c>
-      <c r="AI12" t="s">
-        <v>11</v>
-      </c>
-      <c r="AJ12" t="s">
-        <v>28</v>
-      </c>
-    </row>
-    <row r="13" spans="1:36" x14ac:dyDescent="0.25">
-      <c r="A13" t="s">
+      <c r="D13" t="s">
+        <v>9</v>
+      </c>
+      <c r="G13" t="s">
+        <v>9</v>
+      </c>
+      <c r="AH13" t="s">
+        <v>10</v>
+      </c>
+      <c r="AI13" t="s">
+        <v>11</v>
+      </c>
+      <c r="AJ13" t="s">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="14" spans="1:36" x14ac:dyDescent="0.3">
+      <c r="A14" t="s">
         <v>49</v>
       </c>
-      <c r="D13" t="s">
-        <v>9</v>
-      </c>
-      <c r="G13" t="s">
-        <v>9</v>
-      </c>
-      <c r="AH13" t="s">
-        <v>10</v>
-      </c>
-      <c r="AI13" t="s">
-        <v>11</v>
-      </c>
-      <c r="AJ13" t="s">
-        <v>28</v>
-      </c>
-    </row>
-    <row r="14" spans="1:36" x14ac:dyDescent="0.25">
-      <c r="A14" t="s">
+      <c r="D14" t="s">
+        <v>9</v>
+      </c>
+      <c r="L14" t="s">
+        <v>9</v>
+      </c>
+      <c r="P14" t="s">
+        <v>9</v>
+      </c>
+      <c r="AH14" t="s">
+        <v>10</v>
+      </c>
+      <c r="AI14" t="s">
+        <v>11</v>
+      </c>
+      <c r="AJ14" t="s">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="15" spans="1:36" x14ac:dyDescent="0.3">
+      <c r="A15" t="s">
         <v>50</v>
       </c>
-      <c r="D14" t="s">
-        <v>9</v>
-      </c>
-      <c r="L14" t="s">
-        <v>9</v>
-      </c>
-      <c r="P14" t="s">
-        <v>9</v>
-      </c>
-      <c r="AH14" t="s">
-        <v>10</v>
-      </c>
-      <c r="AI14" t="s">
-        <v>11</v>
-      </c>
-      <c r="AJ14" t="s">
-        <v>28</v>
-      </c>
-    </row>
-    <row r="15" spans="1:36" x14ac:dyDescent="0.25">
-      <c r="A15" t="s">
+      <c r="D15" t="s">
+        <v>9</v>
+      </c>
+      <c r="J15" t="s">
+        <v>9</v>
+      </c>
+      <c r="N15" t="s">
+        <v>9</v>
+      </c>
+      <c r="AH15" t="s">
+        <v>10</v>
+      </c>
+      <c r="AI15" t="s">
+        <v>11</v>
+      </c>
+      <c r="AJ15" t="s">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="16" spans="1:36" x14ac:dyDescent="0.3">
+      <c r="A16" t="s">
         <v>51</v>
       </c>
-      <c r="D15" t="s">
-        <v>9</v>
-      </c>
-      <c r="J15" t="s">
-        <v>9</v>
-      </c>
-      <c r="N15" t="s">
-        <v>9</v>
-      </c>
-      <c r="AH15" t="s">
-        <v>10</v>
-      </c>
-      <c r="AI15" t="s">
-        <v>11</v>
-      </c>
-      <c r="AJ15" t="s">
-        <v>28</v>
-      </c>
-    </row>
-    <row r="16" spans="1:36" x14ac:dyDescent="0.25">
-      <c r="A16" t="s">
+      <c r="D16" t="s">
+        <v>9</v>
+      </c>
+      <c r="K16" t="s">
+        <v>9</v>
+      </c>
+      <c r="O16" t="s">
+        <v>9</v>
+      </c>
+      <c r="AH16" t="s">
+        <v>10</v>
+      </c>
+      <c r="AI16" t="s">
+        <v>11</v>
+      </c>
+      <c r="AJ16" t="s">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="17" spans="1:36" x14ac:dyDescent="0.3">
+      <c r="A17" t="s">
         <v>52</v>
       </c>
-      <c r="D16" t="s">
-        <v>9</v>
-      </c>
-      <c r="K16" t="s">
-        <v>9</v>
-      </c>
-      <c r="O16" t="s">
-        <v>9</v>
-      </c>
-      <c r="AH16" t="s">
-        <v>10</v>
-      </c>
-      <c r="AI16" t="s">
-        <v>11</v>
-      </c>
-      <c r="AJ16" t="s">
-        <v>28</v>
-      </c>
-    </row>
-    <row r="17" spans="1:36" x14ac:dyDescent="0.25">
-      <c r="A17" t="s">
+      <c r="D17" t="s">
+        <v>9</v>
+      </c>
+      <c r="I17" t="s">
+        <v>9</v>
+      </c>
+      <c r="AH17" t="s">
+        <v>10</v>
+      </c>
+      <c r="AI17" t="s">
+        <v>11</v>
+      </c>
+      <c r="AJ17" t="s">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="18" spans="1:36" x14ac:dyDescent="0.3">
+      <c r="A18" t="s">
         <v>53</v>
       </c>
-      <c r="D17" t="s">
-        <v>9</v>
-      </c>
-      <c r="I17" t="s">
-        <v>9</v>
-      </c>
-      <c r="AH17" t="s">
-        <v>10</v>
-      </c>
-      <c r="AI17" t="s">
-        <v>11</v>
-      </c>
-      <c r="AJ17" t="s">
-        <v>28</v>
-      </c>
-    </row>
-    <row r="18" spans="1:36" x14ac:dyDescent="0.25">
-      <c r="A18" t="s">
+      <c r="D18" t="s">
+        <v>9</v>
+      </c>
+      <c r="M18" t="s">
+        <v>9</v>
+      </c>
+      <c r="Q18" t="s">
+        <v>9</v>
+      </c>
+      <c r="AH18" t="s">
+        <v>10</v>
+      </c>
+      <c r="AI18" t="s">
+        <v>11</v>
+      </c>
+      <c r="AJ18" t="s">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="19" spans="1:36" x14ac:dyDescent="0.3">
+      <c r="A19" t="s">
         <v>54</v>
       </c>
-      <c r="D18" t="s">
-        <v>9</v>
-      </c>
-      <c r="M18" t="s">
-        <v>9</v>
-      </c>
-      <c r="Q18" t="s">
-        <v>9</v>
-      </c>
-      <c r="AH18" t="s">
-        <v>10</v>
-      </c>
-      <c r="AI18" t="s">
-        <v>11</v>
-      </c>
-      <c r="AJ18" t="s">
-        <v>28</v>
-      </c>
-    </row>
-    <row r="19" spans="1:36" x14ac:dyDescent="0.25">
-      <c r="A19" t="s">
+      <c r="T19" t="s">
+        <v>9</v>
+      </c>
+      <c r="U19" t="s">
+        <v>9</v>
+      </c>
+      <c r="X19" t="s">
+        <v>9</v>
+      </c>
+      <c r="AH19" t="s">
+        <v>10</v>
+      </c>
+      <c r="AI19" t="s">
+        <v>11</v>
+      </c>
+      <c r="AJ19" t="s">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="20" spans="1:36" x14ac:dyDescent="0.3">
+      <c r="A20" t="s">
         <v>55</v>
       </c>
-      <c r="T19" t="s">
-        <v>9</v>
-      </c>
-      <c r="U19" t="s">
-        <v>9</v>
-      </c>
-      <c r="X19" t="s">
-        <v>9</v>
-      </c>
-      <c r="AH19" t="s">
-        <v>10</v>
-      </c>
-      <c r="AI19" t="s">
-        <v>11</v>
-      </c>
-      <c r="AJ19" t="s">
-        <v>28</v>
-      </c>
-    </row>
-    <row r="20" spans="1:36" x14ac:dyDescent="0.25">
-      <c r="A20" t="s">
+      <c r="T20" t="s">
+        <v>9</v>
+      </c>
+      <c r="U20" t="s">
+        <v>9</v>
+      </c>
+      <c r="V20" t="s">
+        <v>9</v>
+      </c>
+      <c r="AH20" t="s">
+        <v>10</v>
+      </c>
+      <c r="AI20" t="s">
+        <v>11</v>
+      </c>
+      <c r="AJ20" t="s">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="21" spans="1:36" x14ac:dyDescent="0.3">
+      <c r="A21" t="s">
         <v>56</v>
       </c>
-      <c r="T20" t="s">
-        <v>9</v>
-      </c>
-      <c r="U20" t="s">
-        <v>9</v>
-      </c>
-      <c r="V20" t="s">
-        <v>9</v>
-      </c>
-      <c r="AH20" t="s">
-        <v>10</v>
-      </c>
-      <c r="AI20" t="s">
-        <v>11</v>
-      </c>
-      <c r="AJ20" t="s">
-        <v>28</v>
-      </c>
-    </row>
-    <row r="21" spans="1:36" x14ac:dyDescent="0.25">
-      <c r="A21" t="s">
+      <c r="T21" t="s">
+        <v>9</v>
+      </c>
+      <c r="U21" t="s">
+        <v>9</v>
+      </c>
+      <c r="W21" t="s">
+        <v>9</v>
+      </c>
+      <c r="AH21" t="s">
+        <v>10</v>
+      </c>
+      <c r="AI21" t="s">
+        <v>11</v>
+      </c>
+      <c r="AJ21" t="s">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="22" spans="1:36" x14ac:dyDescent="0.3">
+      <c r="A22" t="s">
         <v>57</v>
       </c>
-      <c r="T21" t="s">
-        <v>9</v>
-      </c>
-      <c r="U21" t="s">
-        <v>9</v>
-      </c>
-      <c r="W21" t="s">
-        <v>9</v>
-      </c>
-      <c r="AH21" t="s">
-        <v>10</v>
-      </c>
-      <c r="AI21" t="s">
-        <v>11</v>
-      </c>
-      <c r="AJ21" t="s">
-        <v>28</v>
-      </c>
-    </row>
-    <row r="22" spans="1:36" x14ac:dyDescent="0.25">
-      <c r="A22" t="s">
+      <c r="T22" t="s">
+        <v>9</v>
+      </c>
+      <c r="U22" t="s">
+        <v>9</v>
+      </c>
+      <c r="AB22" t="s">
+        <v>9</v>
+      </c>
+      <c r="AF22" t="s">
+        <v>9</v>
+      </c>
+      <c r="AH22" t="s">
+        <v>10</v>
+      </c>
+      <c r="AI22" t="s">
+        <v>11</v>
+      </c>
+      <c r="AJ22" t="s">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="23" spans="1:36" x14ac:dyDescent="0.3">
+      <c r="A23" t="s">
         <v>58</v>
       </c>
-      <c r="T22" t="s">
-        <v>9</v>
-      </c>
-      <c r="U22" t="s">
-        <v>9</v>
-      </c>
-      <c r="AB22" t="s">
-        <v>9</v>
-      </c>
-      <c r="AF22" t="s">
-        <v>9</v>
-      </c>
-      <c r="AH22" t="s">
-        <v>10</v>
-      </c>
-      <c r="AI22" t="s">
-        <v>11</v>
-      </c>
-      <c r="AJ22" t="s">
-        <v>28</v>
-      </c>
-    </row>
-    <row r="23" spans="1:36" x14ac:dyDescent="0.25">
-      <c r="A23" t="s">
+      <c r="T23" t="s">
+        <v>9</v>
+      </c>
+      <c r="U23" t="s">
+        <v>9</v>
+      </c>
+      <c r="Z23" t="s">
+        <v>9</v>
+      </c>
+      <c r="AD23" t="s">
+        <v>9</v>
+      </c>
+      <c r="AH23" t="s">
+        <v>10</v>
+      </c>
+      <c r="AI23" t="s">
+        <v>11</v>
+      </c>
+      <c r="AJ23" t="s">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="24" spans="1:36" x14ac:dyDescent="0.3">
+      <c r="A24" t="s">
         <v>59</v>
       </c>
-      <c r="T23" t="s">
-        <v>9</v>
-      </c>
-      <c r="U23" t="s">
-        <v>9</v>
-      </c>
-      <c r="Z23" t="s">
-        <v>9</v>
-      </c>
-      <c r="AD23" t="s">
-        <v>9</v>
-      </c>
-      <c r="AH23" t="s">
-        <v>10</v>
-      </c>
-      <c r="AI23" t="s">
-        <v>11</v>
-      </c>
-      <c r="AJ23" t="s">
-        <v>28</v>
-      </c>
-    </row>
-    <row r="24" spans="1:36" x14ac:dyDescent="0.25">
-      <c r="A24" t="s">
+      <c r="T24" t="s">
+        <v>9</v>
+      </c>
+      <c r="U24" t="s">
+        <v>9</v>
+      </c>
+      <c r="AA24" t="s">
+        <v>9</v>
+      </c>
+      <c r="AE24" t="s">
+        <v>9</v>
+      </c>
+      <c r="AH24" t="s">
+        <v>10</v>
+      </c>
+      <c r="AI24" t="s">
+        <v>11</v>
+      </c>
+      <c r="AJ24" t="s">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="25" spans="1:36" x14ac:dyDescent="0.3">
+      <c r="A25" t="s">
         <v>60</v>
       </c>
-      <c r="T24" t="s">
-        <v>9</v>
-      </c>
-      <c r="U24" t="s">
-        <v>9</v>
-      </c>
-      <c r="AA24" t="s">
-        <v>9</v>
-      </c>
-      <c r="AE24" t="s">
-        <v>9</v>
-      </c>
-      <c r="AH24" t="s">
-        <v>10</v>
-      </c>
-      <c r="AI24" t="s">
-        <v>11</v>
-      </c>
-      <c r="AJ24" t="s">
-        <v>28</v>
-      </c>
-    </row>
-    <row r="25" spans="1:36" x14ac:dyDescent="0.25">
-      <c r="A25" t="s">
+      <c r="T25" t="s">
+        <v>9</v>
+      </c>
+      <c r="U25" t="s">
+        <v>9</v>
+      </c>
+      <c r="Y25" t="s">
+        <v>9</v>
+      </c>
+      <c r="AH25" t="s">
+        <v>10</v>
+      </c>
+      <c r="AI25" t="s">
+        <v>11</v>
+      </c>
+      <c r="AJ25" t="s">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="26" spans="1:36" x14ac:dyDescent="0.3">
+      <c r="A26" t="s">
         <v>61</v>
       </c>
-      <c r="T25" t="s">
-        <v>9</v>
-      </c>
-      <c r="U25" t="s">
-        <v>9</v>
-      </c>
-      <c r="Y25" t="s">
-        <v>9</v>
-      </c>
-      <c r="AH25" t="s">
-        <v>10</v>
-      </c>
-      <c r="AI25" t="s">
-        <v>11</v>
-      </c>
-      <c r="AJ25" t="s">
-        <v>28</v>
-      </c>
-    </row>
-    <row r="26" spans="1:36" x14ac:dyDescent="0.25">
-      <c r="A26" t="s">
-        <v>62</v>
-      </c>
       <c r="T26" t="s">
         <v>9</v>
       </c>
@@ -1771,7 +1771,7 @@
         <v>11</v>
       </c>
       <c r="AJ26" t="s">
-        <v>28</v>
+        <v>64</v>
       </c>
     </row>
   </sheetData>

</xml_diff>